<commit_message>
Tạo xong bàn cờ
</commit_message>
<xml_diff>
--- a/Kế-hoạch-game-caro-2-người-chơi.xlsx
+++ b/Kế-hoạch-game-caro-2-người-chơi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tuong be de\Desktop\Cấu trúc dữ liệu và giải thuật\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tuong be de\Desktop\GitHub\game-caro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BDE4D2-AA93-4E47-AE3D-2B51813DDB3D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC31FB6-E843-4706-9357-78CD90761D67}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{9D2AB4CB-00F6-461F-83A4-BBA81D90BC74}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{9D2AB4CB-00F6-461F-83A4-BBA81D90BC74}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="46">
   <si>
     <t>Stt</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Tạo mô hình chung hiển thị cho bàn cờ và anchor</t>
   </si>
   <si>
-    <t>Tạo ra bàn cờ cơ bàn, xây dựng thuật toán tạo bàn cơ khoảng 16*16</t>
-  </si>
-  <si>
     <t>Tạo ra, cho phép người dùng tự đặt tên cho mình nếu muốn</t>
   </si>
   <si>
@@ -160,6 +157,12 @@
   </si>
   <si>
     <t>Làm báo cáo trên word</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tạo ra bàn cờ cơ bàn, xây dựng thuật toán tạo bàn cờ 19x23  </t>
+  </si>
+  <si>
+    <t>08 tháng 10</t>
   </si>
 </sst>
 </file>
@@ -636,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE84ED23-3FAC-42AA-9587-87217D3F8ED7}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,7 +658,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -700,10 +703,10 @@
         <v>17</v>
       </c>
       <c r="H3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -714,14 +717,14 @@
         <v>4</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>33</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>34</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>18</v>
@@ -738,19 +741,23 @@
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>34</v>
-      </c>
       <c r="G5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
+        <v>44</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
@@ -760,17 +767,17 @@
         <v>7</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>34</v>
-      </c>
       <c r="G6" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H6" s="20"/>
       <c r="I6" s="20"/>
@@ -784,16 +791,16 @@
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H7" s="20"/>
       <c r="I7" s="20"/>
@@ -807,16 +814,16 @@
       </c>
       <c r="C8" s="16"/>
       <c r="D8" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H8" s="20"/>
       <c r="I8" s="20"/>
@@ -829,17 +836,17 @@
         <v>10</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
@@ -852,17 +859,17 @@
         <v>11</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
@@ -876,16 +883,16 @@
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
@@ -898,17 +905,17 @@
         <v>13</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" s="16"/>
       <c r="E12" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H12" s="20"/>
       <c r="I12" s="20"/>
@@ -922,16 +929,16 @@
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H13" s="20"/>
       <c r="I13" s="20"/>
@@ -944,19 +951,19 @@
         <v>15</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="11" t="s">
-        <v>40</v>
-      </c>
       <c r="G14" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
@@ -966,29 +973,29 @@
         <v>12</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="18" t="s">
-        <v>40</v>
-      </c>
       <c r="G15" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H15" s="20"/>
       <c r="I15" s="20"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
@@ -996,7 +1003,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>

</xml_diff>

<commit_message>
Xử lí thắng thua
</commit_message>
<xml_diff>
--- a/Kế-hoạch-game-caro-2-người-chơi.xlsx
+++ b/Kế-hoạch-game-caro-2-người-chơi.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thang\Desktop\game-caro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tuong be de\Desktop\GitHub\game-caro\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300CFFC0-3AD7-4982-8DB2-2031F6F2C77B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
   <si>
     <t>Stt</t>
   </si>
@@ -177,12 +178,15 @@
   </si>
   <si>
     <t>19 tháng 10</t>
+  </si>
+  <si>
+    <t>20 tháng 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -650,11 +654,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,8 +855,12 @@
       <c r="G8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
+      <c r="H8" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">

</xml_diff>

<commit_message>
tạo menu và hotkey
</commit_message>
<xml_diff>
--- a/Kế-hoạch-game-caro-2-người-chơi.xlsx
+++ b/Kế-hoạch-game-caro-2-người-chơi.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tuong be de\Desktop\GitHub\game-caro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thang\Desktop\game-caro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300CFFC0-3AD7-4982-8DB2-2031F6F2C77B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="53">
   <si>
     <t>Stt</t>
   </si>
@@ -181,12 +180,15 @@
   </si>
   <si>
     <t>20 tháng 10</t>
+  </si>
+  <si>
+    <t>22 tháng 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -654,11 +656,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,8 +884,12 @@
       <c r="G9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
+      <c r="H9" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3">

</xml_diff>

<commit_message>
Chức năng Undo dùng Stack
</commit_message>
<xml_diff>
--- a/Kế-hoạch-game-caro-2-người-chơi.xlsx
+++ b/Kế-hoạch-game-caro-2-người-chơi.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thang\Desktop\game-caro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tuong be de\Desktop\GitHub\game-caro\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9EBA66E-FC94-480F-AA87-0DEAD7C23728}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
   <si>
     <t>Stt</t>
   </si>
@@ -183,12 +184,15 @@
   </si>
   <si>
     <t>22 tháng 10</t>
+  </si>
+  <si>
+    <t>23 tháng 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -656,11 +660,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,8 +938,12 @@
       <c r="G11" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
+      <c r="H11" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3">

</xml_diff>

<commit_message>
Add class Generic StackCaro
</commit_message>
<xml_diff>
--- a/Kế-hoạch-game-caro-2-người-chơi.xlsx
+++ b/Kế-hoạch-game-caro-2-người-chơi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tuong be de\Desktop\game-caro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2CB1DD-D8F0-4A2F-B4BB-BBD15DBDE7D6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9391835C-31EF-4294-81CA-43D6B222D0DD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
   <si>
     <t>Stt</t>
   </si>
@@ -174,10 +174,13 @@
     <t>23 tháng 10</t>
   </si>
   <si>
-    <t>1 tháng 11</t>
-  </si>
-  <si>
     <t>Tạo ra với image mark riêng cho tường người</t>
+  </si>
+  <si>
+    <t>1 tháng 12</t>
+  </si>
+  <si>
+    <t>6 tháng 12</t>
   </si>
 </sst>
 </file>
@@ -725,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,7 +870,7 @@
         <v>28</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H6" s="19" t="s">
         <v>33</v>
@@ -1030,9 +1033,11 @@
         <v>21</v>
       </c>
       <c r="H12" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="I12" s="19"/>
+        <v>50</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="16">

</xml_diff>